<commit_message>
Weekly update, memory done
</commit_message>
<xml_diff>
--- a/report/sadman.xlsx
+++ b/report/sadman.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sadma\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{231833C4-B28D-49CB-8635-C2AA3125EEBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{622F801A-D46D-4453-B587-E867A186CAE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{9F76B2F9-286B-4066-94AA-47694711870D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Till 03/13/25</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>Was able to use and access the FPGA sdram controller. Seemed to work fine when tested manually but still some inconsistencies when accessing sequentially. Tried to implement the axi bridge and access HPS sdram but having few issues. Need to discuss with team and TA/instructor.</t>
+  </si>
+  <si>
+    <t>Created a qsys setup with hps and dma controllers but seemed like accessing the hps using Linux was not a viable option. So, changed plan to use the FPGA Sdram instead and use JTAG master to load up memory from external pc. Also creadted a custom IP named SDRAM_Wrapper and connected in QSYS that can be used in other modules to rd/wr from sdram. So, Memory part of the project is done, just need to integrated with design.</t>
   </si>
 </sst>
 </file>
@@ -103,7 +106,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -114,7 +117,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -449,15 +451,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90CE2574-222C-4AFC-949F-167DB0C45B69}">
-  <dimension ref="A1:W18"/>
+  <dimension ref="A1:AM18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="Y4" sqref="Y4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -470,7 +472,7 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -483,7 +485,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>45734</v>
       </c>
@@ -492,7 +494,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>45747</v>
       </c>
@@ -521,32 +523,52 @@
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
+    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>45760</v>
+      </c>
       <c r="B5" s="1"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="4"/>
-      <c r="S5" s="4"/>
-      <c r="T5" s="4"/>
-      <c r="U5" s="4"/>
-      <c r="V5" s="4"/>
-      <c r="W5" s="4"/>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1"/>
+      <c r="AA5" s="1"/>
+      <c r="AB5" s="1"/>
+      <c r="AC5" s="1"/>
+      <c r="AD5" s="1"/>
+      <c r="AE5" s="1"/>
+      <c r="AF5" s="1"/>
+      <c r="AG5" s="1"/>
+      <c r="AH5" s="1"/>
+      <c r="AI5" s="1"/>
+      <c r="AJ5" s="1"/>
+      <c r="AK5" s="1"/>
+      <c r="AL5" s="1"/>
+      <c r="AM5" s="1"/>
+    </row>
+    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -555,7 +577,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -564,7 +586,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -573,7 +595,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -582,7 +604,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -591,7 +613,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -600,7 +622,7 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -609,7 +631,7 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -618,7 +640,7 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -627,7 +649,7 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -636,7 +658,7 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -664,7 +686,7 @@
       <c r="G18" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="34">
+  <mergeCells count="35">
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
@@ -675,6 +697,7 @@
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="C4:W4"/>
+    <mergeCell ref="C5:AM5"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="C2:G2"/>
     <mergeCell ref="C6:G6"/>

</xml_diff>